<commit_message>
update skills and project
</commit_message>
<xml_diff>
--- a/assets/data/Project.xlsx
+++ b/assets/data/Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Web\personal-web\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Web\personal-web\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058A26E2-3B13-4594-8685-A9398B3B2B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1C8C1E-3D31-4475-A651-8882E185DC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{007D2C89-13C6-402C-A6C9-47ED4AE51617}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{007D2C89-13C6-402C-A6C9-47ED4AE51617}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Project Name</t>
   </si>
@@ -60,29 +60,75 @@
     <t>Developer</t>
   </si>
   <si>
-    <t>Coursework - Github</t>
-  </si>
-  <si>
     <t>House Prices</t>
   </si>
   <si>
-    <t>Kaggle Competition</t>
-  </si>
-  <si>
     <t>Spaceship Titanic</t>
   </si>
   <si>
-    <t>Kaggle Competitons</t>
-  </si>
-  <si>
     <t>Image Processing</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Sharpen, blurred, segmentation, boundary extraction, feature extraction image(s) by many techniques with GUI</t>
+  </si>
+  <si>
+    <t>Stroke disease prediction using SVM, Decision Tree, MLP with GUI.</t>
+  </si>
+  <si>
+    <t>Predict which passengers are transported to an alternate dimension.</t>
+  </si>
+  <si>
+    <t>Predict the sales price for each house.</t>
+  </si>
+  <si>
+    <t>Digit Recognizer</t>
+  </si>
+  <si>
+    <t>Correctly identify digits from a dataset of tens of thousands of handwritten images(MNIST).</t>
+  </si>
+  <si>
+    <t>CringeMPOne</t>
+  </si>
+  <si>
+    <t>Developing member</t>
+  </si>
+  <si>
+    <t>Music streaming application inspired by ZingMP3.
+My role: Developing song search functionality, connecting, and storing user data on Firebase.</t>
+  </si>
+  <si>
+    <t>Family Tree</t>
+  </si>
+  <si>
+    <t>FamilyTree</t>
+  </si>
+  <si>
+    <t>Digit-Recognizer</t>
+  </si>
+  <si>
+    <t>HousePrices</t>
+  </si>
+  <si>
+    <t>SpaceshipTitanic</t>
+  </si>
+  <si>
+    <t>StrokePrediction</t>
+  </si>
+  <si>
+    <t>ImageProcessing</t>
+  </si>
+  <si>
+    <t>The project involves building a family tree application using Java and Neo4j.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +145,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,11 +178,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617A40F4-C719-4F1E-B1F8-7642E9714DFC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -460,7 +520,7 @@
     <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -476,27 +536,33 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>2023</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7FE49667-796D-4368-A0C7-1ECF267D59B2}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6C249173-46DD-4297-A84B-E6969D632B58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -505,10 +571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DAE04E-7E7D-4B5B-88B9-4D777C0B7A50}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -518,9 +584,10 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -536,13 +603,16 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -550,33 +620,39 @@
       <c r="D2">
         <v>2023</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
         <v>2023</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -584,20 +660,86 @@
       <c r="D4">
         <v>2023</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="129.6">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>2023</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>2023</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>2023</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E3">
-    <sortCondition descending="1" ref="D2:D3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E6">
+    <sortCondition descending="1" ref="D4:D6"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{5AD5DC24-0035-4EFD-BA2A-CE1933DAF1B2}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00DF741A-1B4A-42D7-82BC-C0053F8AA57D}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{9DDBA80F-C826-4FA5-80A4-0FA03179237B}"/>
+    <hyperlink ref="F6" r:id="rId1" display="Coursework - Github" xr:uid="{5AD5DC24-0035-4EFD-BA2A-CE1933DAF1B2}"/>
+    <hyperlink ref="F4" r:id="rId2" display="Kaggle Competitons" xr:uid="{00DF741A-1B4A-42D7-82BC-C0053F8AA57D}"/>
+    <hyperlink ref="F7" r:id="rId3" display="Coursework - Github" xr:uid="{9DDBA80F-C826-4FA5-80A4-0FA03179237B}"/>
+    <hyperlink ref="F3" r:id="rId4" display="Kaggle Competition" xr:uid="{794EBAEA-652C-4115-96E3-393F9DED0446}"/>
+    <hyperlink ref="F2" r:id="rId5" display="https://github.com/nguyen378/Digit-Recognizer" xr:uid="{934B3E95-77D8-422B-905B-B4106F49D18A}"/>
+    <hyperlink ref="F5" r:id="rId6" display="https://github.com/dat911zz/CringeMPOne" xr:uid="{15470452-9858-46CE-86D2-75428DAAB37A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CV and project
</commit_message>
<xml_diff>
--- a/assets/data/Project.xlsx
+++ b/assets/data/Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\Web\personal-web\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7F0BBF-0AC1-4E45-96C3-A5A6FA00FB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40DA56E-FAF5-46F0-B740-BAB3CCB51518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{007D2C89-13C6-402C-A6C9-47ED4AE51617}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{007D2C89-13C6-402C-A6C9-47ED4AE51617}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Project Name</t>
   </si>
@@ -135,7 +135,31 @@
     <t>SecureMemo</t>
   </si>
   <si>
-    <t>SmartTrafic</t>
+    <t>Traffic light optimization based on vehicle traffic density</t>
+  </si>
+  <si>
+    <t>Using the YOLOv10 model to classify vehicle traffic density, thereby applying a formula to calculate the time difference between routes.</t>
+  </si>
+  <si>
+    <t>nguyen378/Thesis</t>
+  </si>
+  <si>
+    <t>nguyen378/MyLifeManager (github.com)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/2024 - ? </t>
+  </si>
+  <si>
+    <t>MyLifeManager( Font-end)</t>
+  </si>
+  <si>
+    <t>MyLifeManager( Back-end)</t>
+  </si>
+  <si>
+    <t>8/2024 - ?</t>
+  </si>
+  <si>
+    <t>nguyen378/MyLifeManage_Backend (github.com)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -204,6 +228,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -223,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,7 +300,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -369,7 +406,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,20 +556,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617A40F4-C719-4F1E-B1F8-7642E9714DFC}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -560,33 +597,57 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>2024</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://github.com/nguyen378/MyLifeManager" xr:uid="{F5DA71CE-D4F9-4465-889B-0FEFAFFD8FE0}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://github.com/nguyen378/MyLifeManage_Backend" xr:uid="{5C0B4E8B-3B6D-4723-A60A-8426C9E832CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DAE04E-7E7D-4B5B-88B9-4D777C0B7A50}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="92.6640625" bestFit="1" customWidth="1"/>
@@ -615,30 +676,30 @@
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="1">
-        <v>2023</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>2024</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -647,38 +708,38 @@
         <v>2023</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>2023</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -687,18 +748,18 @@
         <v>2023</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -707,87 +768,108 @@
         <v>2023</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>2023</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="1">
         <v>2023</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>2023</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:E8">
-    <sortCondition descending="1" ref="D6:D8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E9">
+    <sortCondition descending="1" ref="D7:D9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="Coursework - Github" xr:uid="{5AD5DC24-0035-4EFD-BA2A-CE1933DAF1B2}"/>
-    <hyperlink ref="F6" r:id="rId2" display="Kaggle Competitons" xr:uid="{00DF741A-1B4A-42D7-82BC-C0053F8AA57D}"/>
-    <hyperlink ref="F9" r:id="rId3" display="Coursework - Github" xr:uid="{9DDBA80F-C826-4FA5-80A4-0FA03179237B}"/>
-    <hyperlink ref="F5" r:id="rId4" display="Kaggle Competition" xr:uid="{794EBAEA-652C-4115-96E3-393F9DED0446}"/>
-    <hyperlink ref="F7" r:id="rId5" display="https://github.com/dat911zz/CringeMPOne" xr:uid="{15470452-9858-46CE-86D2-75428DAAB37A}"/>
-    <hyperlink ref="F4" r:id="rId6" display="https://github.com/nguyen378/Digit-Recognizer" xr:uid="{934B3E95-77D8-422B-905B-B4106F49D18A}"/>
-    <hyperlink ref="F3" r:id="rId7" xr:uid="{6C249173-46DD-4297-A84B-E6969D632B58}"/>
-    <hyperlink ref="F2" r:id="rId8" xr:uid="{208E3FC3-46BC-4C64-B6AE-1C1BFBBF25D2}"/>
+    <hyperlink ref="F9" r:id="rId1" display="Coursework - Github" xr:uid="{5AD5DC24-0035-4EFD-BA2A-CE1933DAF1B2}"/>
+    <hyperlink ref="F7" r:id="rId2" display="Kaggle Competitons" xr:uid="{00DF741A-1B4A-42D7-82BC-C0053F8AA57D}"/>
+    <hyperlink ref="F10" r:id="rId3" display="Coursework - Github" xr:uid="{9DDBA80F-C826-4FA5-80A4-0FA03179237B}"/>
+    <hyperlink ref="F6" r:id="rId4" display="Kaggle Competition" xr:uid="{794EBAEA-652C-4115-96E3-393F9DED0446}"/>
+    <hyperlink ref="F8" r:id="rId5" display="https://github.com/dat911zz/CringeMPOne" xr:uid="{15470452-9858-46CE-86D2-75428DAAB37A}"/>
+    <hyperlink ref="F5" r:id="rId6" display="https://github.com/nguyen378/Digit-Recognizer" xr:uid="{934B3E95-77D8-422B-905B-B4106F49D18A}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{6C249173-46DD-4297-A84B-E6969D632B58}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{208E3FC3-46BC-4C64-B6AE-1C1BFBBF25D2}"/>
+    <hyperlink ref="F2" r:id="rId9" display="https://github.com/nguyen378/Thesis" xr:uid="{D0592AA4-3469-490C-AD0C-57131D02AB44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>